<commit_message>
Added All Java and Excel File
</commit_message>
<xml_diff>
--- a/DemoForPractice/ExcelTestData/TestData.xlsx
+++ b/DemoForPractice/ExcelTestData/TestData.xlsx
@@ -4,20 +4,23 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15060" windowHeight="6435"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15060" windowHeight="6435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="WorkFlowData" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="EmpDetails" sheetId="3" r:id="rId3"/>
+    <sheet name="EmpDetails1" sheetId="4" r:id="rId4"/>
+    <sheet name="EmpDetails2" r:id="rId8" sheetId="5"/>
+    <sheet name="EmpDetails3" r:id="rId9" sheetId="6"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:O20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Env</t>
   </si>
@@ -65,12 +68,19 @@
   </si>
   <si>
     <t>https://pizzaonline.dominos.co.in/menu</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -398,17 +408,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -530,12 +540,74 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>